<commit_message>
Updated for new ST HAL drivers. Added relay on hardware and some other hw updates
</commit_message>
<xml_diff>
--- a/01_Doc/IO.xlsx
+++ b/01_Doc/IO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t>Arduino
 connector</t>
@@ -94,9 +94,6 @@
     <t>LimSW</t>
   </si>
   <si>
-    <t>Limit switch</t>
-  </si>
-  <si>
     <t>CN8-5</t>
   </si>
   <si>
@@ -141,6 +138,60 @@
   </si>
   <si>
     <t>CN7-38</t>
+  </si>
+  <si>
+    <t>CN7-35</t>
+  </si>
+  <si>
+    <t>PC2</t>
+  </si>
+  <si>
+    <t>Selection</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>CN7-37</t>
+  </si>
+  <si>
+    <t>PC3</t>
+  </si>
+  <si>
+    <t>Gas Heater Start</t>
+  </si>
+  <si>
+    <t>CN10-3</t>
+  </si>
+  <si>
+    <t>CN10-5</t>
+  </si>
+  <si>
+    <t>D15</t>
+  </si>
+  <si>
+    <t>D14</t>
+  </si>
+  <si>
+    <t>PB8</t>
+  </si>
+  <si>
+    <t>PB9</t>
+  </si>
+  <si>
+    <t>I2C1_SCL</t>
+  </si>
+  <si>
+    <t>I2C1_SDA</t>
+  </si>
+  <si>
+    <t>Temp Sensor</t>
+  </si>
+  <si>
+    <t>CN5-10</t>
+  </si>
+  <si>
+    <t>CN5-9</t>
   </si>
 </sst>
 </file>
@@ -222,8 +273,8 @@
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>485775</xdr:colOff>
           <xdr:row>43</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
@@ -253,23 +304,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -577,17 +615,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:I8"/>
+  <dimension ref="C3:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -605,7 +643,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>3</v>
@@ -616,30 +654,30 @@
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -651,7 +689,7 @@
         <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
         <v>9</v>
@@ -662,7 +700,7 @@
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -674,7 +712,7 @@
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>
@@ -685,10 +723,10 @@
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -697,21 +735,18 @@
         <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
       </c>
-      <c r="I7" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
@@ -720,13 +755,81 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
       </c>
-      <c r="I8" t="s">
-        <v>21</v>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -747,8 +850,8 @@
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>12</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>11</xdr:col>
+                <xdr:colOff>485775</xdr:colOff>
                 <xdr:row>43</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
Added one input and one output (opto+relay). Use for Start/Selection and Main Heater Control.
</commit_message>
<xml_diff>
--- a/01_Doc/IO.xlsx
+++ b/01_Doc/IO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>Arduino
 connector</t>
@@ -192,6 +192,18 @@
   </si>
   <si>
     <t>CN5-9</t>
+  </si>
+  <si>
+    <t>Usr_Btn_3</t>
+  </si>
+  <si>
+    <t>Usr_Btn_2</t>
+  </si>
+  <si>
+    <t>Usr_Btn_1</t>
+  </si>
+  <si>
+    <t>SW var name</t>
   </si>
 </sst>
 </file>
@@ -274,7 +286,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>485775</xdr:colOff>
+          <xdr:colOff>438150</xdr:colOff>
           <xdr:row>43</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
@@ -615,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:I12"/>
+  <dimension ref="C3:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,9 +639,10 @@
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
@@ -651,8 +664,11 @@
       <c r="I3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>31</v>
       </c>
@@ -675,7 +691,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>32</v>
       </c>
@@ -697,8 +713,11 @@
       <c r="I5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>33</v>
       </c>
@@ -720,8 +739,11 @@
       <c r="I6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>34</v>
       </c>
@@ -741,7 +763,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>35</v>
       </c>
@@ -761,7 +783,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>36</v>
       </c>
@@ -777,8 +799,11 @@
       <c r="I9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>40</v>
       </c>
@@ -792,7 +817,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>43</v>
       </c>
@@ -812,7 +837,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>44</v>
       </c>
@@ -851,7 +876,7 @@
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>485775</xdr:colOff>
+                <xdr:colOff>438150</xdr:colOff>
                 <xdr:row>43</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>

</xml_diff>